<commit_message>
redid author affiliation data, based on PMIDs and finally ran program 7
</commit_message>
<xml_diff>
--- a/2021.09.23 Publications.xlsx
+++ b/2021.09.23 Publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\SNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4D5F89-4CC3-4B14-849A-EA4B8E797975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E7C871-A3EC-4FB1-84CF-F4A5E687B647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="105" windowWidth="14025" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10410" yWindow="300" windowWidth="14025" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal Articles" sheetId="1" r:id="rId1"/>
@@ -1755,6 +1755,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31F722AF-0261-4634-82C0-D16F4EA0FC41}" name="Table1" displayName="Table1" ref="A1:AO26" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:AO26" xr:uid="{31F722AF-0261-4634-82C0-D16F4EA0FC41}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO26">
+    <sortCondition ref="AJ1:AJ26"/>
+  </sortState>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{8ED1A78B-0755-43DC-B8C2-490469D6B5CF}" name="proj_num"/>
     <tableColumn id="2" xr3:uid="{FD965AFA-4FB3-453B-91BB-C0BA9026A27C}" name="date_id" dataDxfId="1"/>
@@ -2283,7 +2286,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3">
         <v>44427</v>
@@ -2304,7 +2307,7 @@
         <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
@@ -2313,67 +2316,67 @@
         <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>241</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="M2" t="s">
-        <v>46</v>
+        <v>243</v>
       </c>
       <c r="N2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>238</v>
+      </c>
+      <c r="P2" t="s">
+        <v>244</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>245</v>
       </c>
       <c r="R2" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" t="s">
-        <v>52</v>
+        <v>247</v>
+      </c>
+      <c r="T2" t="s">
+        <v>248</v>
       </c>
       <c r="W2">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="X2" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="Y2" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
       <c r="Z2" t="s">
-        <v>55</v>
+        <v>251</v>
       </c>
       <c r="AA2" t="s">
-        <v>56</v>
+        <v>252</v>
       </c>
       <c r="AB2" t="s">
-        <v>57</v>
+        <v>253</v>
       </c>
       <c r="AC2" t="s">
-        <v>58</v>
+        <v>254</v>
       </c>
       <c r="AD2" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="AI2" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="AJ2" s="6">
-        <v>33861978</v>
+        <v>33228253</v>
       </c>
       <c r="AK2" t="s">
-        <v>61</v>
+        <v>245</v>
       </c>
       <c r="AL2" t="s">
         <v>62</v>
@@ -2385,27 +2388,27 @@
         <v>64</v>
       </c>
       <c r="AO2" t="s">
-        <v>65</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="B3" s="3">
-        <v>44427</v>
+        <v>44461</v>
       </c>
       <c r="C3" s="3">
         <v>44635</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
@@ -2420,67 +2423,64 @@
         <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="N3">
         <v>2021</v>
       </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="Q3" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="R3" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="S3" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="U3" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="V3" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="W3">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="X3" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="Y3" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="Z3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AB3" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="AC3" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD3" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="AI3" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="AJ3" s="6">
-        <v>33929934</v>
+        <v>33323475</v>
       </c>
       <c r="AK3" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="AL3" t="s">
         <v>62</v>
@@ -2492,12 +2492,12 @@
         <v>64</v>
       </c>
       <c r="AO3" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>272</v>
       </c>
       <c r="B4" s="3">
         <v>44427</v>
@@ -2521,76 +2521,61 @@
         <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
         <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>99</v>
+        <v>273</v>
       </c>
       <c r="L4" t="s">
-        <v>100</v>
+        <v>274</v>
       </c>
       <c r="M4" t="s">
-        <v>101</v>
+        <v>275</v>
       </c>
       <c r="N4">
         <v>2021</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="P4" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="Q4" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="R4" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="S4" t="s">
-        <v>102</v>
-      </c>
-      <c r="U4" t="s">
-        <v>105</v>
-      </c>
-      <c r="V4" t="s">
-        <v>106</v>
-      </c>
-      <c r="W4">
-        <v>8</v>
+        <v>74</v>
+      </c>
+      <c r="T4" t="s">
+        <v>276</v>
       </c>
       <c r="X4" t="s">
-        <v>107</v>
+        <v>277</v>
       </c>
       <c r="Y4" t="s">
-        <v>108</v>
+        <v>278</v>
       </c>
       <c r="Z4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="AB4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>113</v>
+        <v>279</v>
       </c>
       <c r="AI4" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="AJ4" s="6">
-        <v>34092431</v>
+        <v>33471114</v>
       </c>
       <c r="AK4" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="AL4" t="s">
         <v>62</v>
@@ -2602,12 +2587,12 @@
         <v>64</v>
       </c>
       <c r="AO4" t="s">
-        <v>115</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>281</v>
       </c>
       <c r="B5" s="3">
         <v>44427</v>
@@ -2628,7 +2613,7 @@
         <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
         <v>43</v>
@@ -2637,67 +2622,67 @@
         <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>423</v>
       </c>
       <c r="L5" t="s">
-        <v>118</v>
+        <v>424</v>
       </c>
       <c r="M5" t="s">
-        <v>119</v>
+        <v>425</v>
       </c>
       <c r="N5">
         <v>2021</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P5" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="Q5" t="s">
-        <v>120</v>
+        <v>426</v>
       </c>
       <c r="R5" t="s">
-        <v>121</v>
+        <v>258</v>
       </c>
       <c r="S5" t="s">
-        <v>50</v>
-      </c>
-      <c r="T5" t="s">
-        <v>122</v>
+        <v>155</v>
+      </c>
+      <c r="U5" t="s">
+        <v>427</v>
+      </c>
+      <c r="V5" t="s">
+        <v>428</v>
       </c>
       <c r="W5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X5" t="s">
-        <v>123</v>
+        <v>429</v>
       </c>
       <c r="Y5" t="s">
-        <v>124</v>
+        <v>430</v>
       </c>
       <c r="Z5" t="s">
         <v>125</v>
       </c>
       <c r="AB5" t="s">
-        <v>126</v>
+        <v>431</v>
       </c>
       <c r="AC5" t="s">
-        <v>127</v>
+        <v>432</v>
       </c>
       <c r="AD5" t="s">
-        <v>128</v>
+        <v>433</v>
       </c>
       <c r="AI5" t="s">
-        <v>129</v>
+        <v>434</v>
       </c>
       <c r="AJ5" s="6">
-        <v>34143195</v>
+        <v>33577743</v>
       </c>
       <c r="AK5" t="s">
-        <v>130</v>
+        <v>435</v>
       </c>
       <c r="AL5" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="AM5" t="s">
         <v>63</v>
@@ -2706,27 +2691,27 @@
         <v>64</v>
       </c>
       <c r="AO5" t="s">
-        <v>131</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3">
-        <v>44461</v>
+        <v>44427</v>
       </c>
       <c r="C6" s="3">
         <v>44635</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>43</v>
@@ -2735,70 +2720,73 @@
         <v>67</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
         <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
+        <v>297</v>
       </c>
       <c r="L6" t="s">
-        <v>134</v>
+        <v>298</v>
       </c>
       <c r="M6" t="s">
-        <v>135</v>
+        <v>299</v>
       </c>
       <c r="N6">
         <v>2021</v>
       </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>300</v>
       </c>
       <c r="Q6" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="R6" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="S6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="U6" t="s">
-        <v>139</v>
+        <v>301</v>
       </c>
       <c r="V6" t="s">
-        <v>140</v>
+        <v>302</v>
       </c>
       <c r="W6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X6" t="s">
-        <v>141</v>
+        <v>303</v>
       </c>
       <c r="Y6" t="s">
-        <v>142</v>
+        <v>304</v>
       </c>
       <c r="Z6" t="s">
-        <v>143</v>
+        <v>305</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>306</v>
       </c>
       <c r="AB6" t="s">
-        <v>144</v>
+        <v>307</v>
       </c>
       <c r="AC6" t="s">
-        <v>145</v>
+        <v>308</v>
       </c>
       <c r="AD6" t="s">
-        <v>146</v>
+        <v>309</v>
       </c>
       <c r="AI6" t="s">
-        <v>147</v>
+        <v>92</v>
       </c>
       <c r="AJ6" s="6">
-        <v>33323475</v>
+        <v>33764497</v>
       </c>
       <c r="AK6" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="AL6" t="s">
         <v>62</v>
@@ -2810,15 +2798,15 @@
         <v>64</v>
       </c>
       <c r="AO6" t="s">
-        <v>148</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="B7" s="3">
-        <v>44449</v>
+        <v>44427</v>
       </c>
       <c r="C7" s="3">
         <v>44635</v>
@@ -2845,67 +2833,70 @@
         <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="L7" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
       <c r="M7" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="N7">
         <v>2021</v>
       </c>
       <c r="O7" t="s">
-        <v>153</v>
-      </c>
-      <c r="P7" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="Q7" t="s">
-        <v>154</v>
+        <v>208</v>
       </c>
       <c r="R7" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="S7" t="s">
-        <v>155</v>
-      </c>
-      <c r="T7" t="s">
-        <v>156</v>
+        <v>50</v>
+      </c>
+      <c r="U7" t="s">
+        <v>210</v>
+      </c>
+      <c r="V7" t="s">
+        <v>211</v>
       </c>
       <c r="W7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X7" t="s">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="Y7" t="s">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="Z7" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="AB7" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="AC7" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="AD7" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="AE7" t="s">
-        <v>163</v>
+        <v>218</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>219</v>
       </c>
       <c r="AI7" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="AJ7" s="6">
-        <v>34264327</v>
+        <v>33775510</v>
       </c>
       <c r="AK7" t="s">
-        <v>165</v>
+        <v>221</v>
       </c>
       <c r="AL7" t="s">
         <v>62</v>
@@ -2917,15 +2908,15 @@
         <v>64</v>
       </c>
       <c r="AO7" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
       <c r="B8" s="3">
-        <v>44427</v>
+        <v>44440</v>
       </c>
       <c r="C8" s="3">
         <v>44635</v>
@@ -2940,82 +2931,73 @@
         <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
         <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
         <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="L8" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="M8" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="N8">
         <v>2021</v>
       </c>
       <c r="O8" t="s">
-        <v>171</v>
-      </c>
-      <c r="P8" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="Q8" t="s">
-        <v>172</v>
+        <v>227</v>
       </c>
       <c r="R8" t="s">
-        <v>155</v>
-      </c>
-      <c r="S8" t="s">
-        <v>173</v>
-      </c>
-      <c r="T8" t="s">
-        <v>174</v>
+        <v>228</v>
+      </c>
+      <c r="U8" t="s">
+        <v>137</v>
+      </c>
+      <c r="V8" t="s">
+        <v>229</v>
       </c>
       <c r="W8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X8" t="s">
-        <v>175</v>
+        <v>230</v>
       </c>
       <c r="Y8" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="Z8" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="AA8" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="AB8" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>180</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
       <c r="AI8" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
       <c r="AJ8" s="6">
-        <v>34081608</v>
+        <v>33812965</v>
       </c>
       <c r="AK8" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
       <c r="AL8" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="AM8" t="s">
         <v>63</v>
@@ -3024,27 +3006,27 @@
         <v>64</v>
       </c>
       <c r="AO8" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
-        <v>44461</v>
+        <v>44427</v>
       </c>
       <c r="C9" s="3">
         <v>44635</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
         <v>43</v>
@@ -3059,67 +3041,73 @@
         <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>185</v>
+        <v>394</v>
       </c>
       <c r="L9" t="s">
-        <v>186</v>
+        <v>395</v>
       </c>
       <c r="M9" t="s">
-        <v>187</v>
+        <v>396</v>
       </c>
       <c r="N9">
         <v>2021</v>
       </c>
       <c r="O9" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="Q9" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="R9" t="s">
-        <v>190</v>
+        <v>91</v>
       </c>
       <c r="S9" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="U9" t="s">
-        <v>191</v>
+        <v>397</v>
       </c>
       <c r="V9" t="s">
-        <v>192</v>
+        <v>398</v>
+      </c>
+      <c r="W9">
+        <v>15</v>
       </c>
       <c r="X9" t="s">
-        <v>193</v>
+        <v>399</v>
       </c>
       <c r="Y9" t="s">
-        <v>194</v>
+        <v>400</v>
       </c>
       <c r="Z9" t="s">
-        <v>195</v>
+        <v>401</v>
       </c>
       <c r="AA9" t="s">
-        <v>196</v>
+        <v>402</v>
       </c>
       <c r="AB9" t="s">
-        <v>197</v>
+        <v>403</v>
       </c>
       <c r="AC9" t="s">
-        <v>198</v>
+        <v>404</v>
       </c>
       <c r="AD9" t="s">
-        <v>199</v>
+        <v>405</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>406</v>
       </c>
       <c r="AI9" t="s">
-        <v>200</v>
+        <v>92</v>
       </c>
       <c r="AJ9" s="6">
-        <v>34159841</v>
+        <v>33861873</v>
       </c>
       <c r="AK9" t="s">
-        <v>201</v>
+        <v>93</v>
       </c>
       <c r="AL9" t="s">
-        <v>202</v>
+        <v>62</v>
       </c>
       <c r="AM9" t="s">
         <v>63</v>
@@ -3128,12 +3116,12 @@
         <v>64</v>
       </c>
       <c r="AO9" t="s">
-        <v>203</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3">
         <v>44427</v>
@@ -3154,7 +3142,7 @@
         <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="I10" t="s">
         <v>43</v>
@@ -3163,13 +3151,13 @@
         <v>43</v>
       </c>
       <c r="K10" t="s">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
-        <v>206</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>207</v>
+        <v>46</v>
       </c>
       <c r="N10">
         <v>2021</v>
@@ -3178,55 +3166,52 @@
         <v>47</v>
       </c>
       <c r="Q10" t="s">
-        <v>208</v>
+        <v>48</v>
       </c>
       <c r="R10" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="S10" t="s">
         <v>50</v>
       </c>
       <c r="U10" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="V10" t="s">
-        <v>211</v>
+        <v>52</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="X10" t="s">
-        <v>212</v>
+        <v>53</v>
       </c>
       <c r="Y10" t="s">
-        <v>213</v>
+        <v>54</v>
       </c>
       <c r="Z10" t="s">
-        <v>214</v>
+        <v>55</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>56</v>
       </c>
       <c r="AB10" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="AC10" t="s">
-        <v>216</v>
+        <v>58</v>
       </c>
       <c r="AD10" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>218</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="AI10" t="s">
-        <v>220</v>
+        <v>60</v>
       </c>
       <c r="AJ10" s="6">
-        <v>33775510</v>
+        <v>33861978</v>
       </c>
       <c r="AK10" t="s">
-        <v>221</v>
+        <v>61</v>
       </c>
       <c r="AL10" t="s">
         <v>62</v>
@@ -3238,15 +3223,15 @@
         <v>64</v>
       </c>
       <c r="AO10" t="s">
-        <v>222</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B11" s="3">
-        <v>44440</v>
+        <v>44427</v>
       </c>
       <c r="C11" s="3">
         <v>44635</v>
@@ -3261,70 +3246,82 @@
         <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s">
         <v>43</v>
       </c>
       <c r="K11" t="s">
-        <v>224</v>
+        <v>363</v>
       </c>
       <c r="L11" t="s">
-        <v>225</v>
+        <v>364</v>
       </c>
       <c r="M11" t="s">
-        <v>226</v>
+        <v>365</v>
       </c>
       <c r="N11">
         <v>2021</v>
       </c>
       <c r="O11" t="s">
-        <v>153</v>
+        <v>300</v>
+      </c>
+      <c r="P11" t="s">
+        <v>204</v>
       </c>
       <c r="Q11" t="s">
-        <v>227</v>
+        <v>366</v>
       </c>
       <c r="R11" t="s">
-        <v>228</v>
+        <v>138</v>
+      </c>
+      <c r="S11" t="s">
+        <v>132</v>
       </c>
       <c r="U11" t="s">
-        <v>137</v>
+        <v>367</v>
       </c>
       <c r="V11" t="s">
-        <v>229</v>
+        <v>368</v>
       </c>
       <c r="W11">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="X11" t="s">
-        <v>230</v>
+        <v>369</v>
       </c>
       <c r="Y11" t="s">
-        <v>231</v>
+        <v>370</v>
       </c>
       <c r="Z11" t="s">
-        <v>232</v>
+        <v>371</v>
       </c>
       <c r="AA11" t="s">
-        <v>233</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>234</v>
+        <v>372</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>373</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>374</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>375</v>
       </c>
       <c r="AI11" t="s">
-        <v>235</v>
+        <v>376</v>
       </c>
       <c r="AJ11" s="6">
-        <v>33812965</v>
+        <v>33870242</v>
       </c>
       <c r="AK11" t="s">
-        <v>236</v>
+        <v>377</v>
       </c>
       <c r="AL11" t="s">
         <v>62</v>
@@ -3336,12 +3333,12 @@
         <v>64</v>
       </c>
       <c r="AO11" t="s">
-        <v>237</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>66</v>
       </c>
       <c r="B12" s="3">
         <v>44427</v>
@@ -3371,67 +3368,67 @@
         <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>241</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>242</v>
+        <v>69</v>
       </c>
       <c r="M12" t="s">
-        <v>243</v>
+        <v>70</v>
       </c>
       <c r="N12">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="O12" t="s">
-        <v>238</v>
-      </c>
-      <c r="P12" t="s">
-        <v>244</v>
+        <v>71</v>
       </c>
       <c r="Q12" t="s">
-        <v>245</v>
+        <v>72</v>
       </c>
       <c r="R12" t="s">
-        <v>246</v>
+        <v>73</v>
       </c>
       <c r="S12" t="s">
-        <v>247</v>
-      </c>
-      <c r="T12" t="s">
-        <v>248</v>
+        <v>74</v>
+      </c>
+      <c r="U12" t="s">
+        <v>75</v>
+      </c>
+      <c r="V12" t="s">
+        <v>76</v>
       </c>
       <c r="W12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X12" t="s">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="Y12" t="s">
-        <v>250</v>
+        <v>78</v>
       </c>
       <c r="Z12" t="s">
-        <v>251</v>
+        <v>79</v>
       </c>
       <c r="AA12" t="s">
-        <v>252</v>
+        <v>80</v>
       </c>
       <c r="AB12" t="s">
-        <v>253</v>
+        <v>81</v>
       </c>
       <c r="AC12" t="s">
-        <v>254</v>
+        <v>82</v>
       </c>
       <c r="AD12" t="s">
-        <v>255</v>
+        <v>83</v>
       </c>
       <c r="AI12" t="s">
-        <v>256</v>
+        <v>84</v>
       </c>
       <c r="AJ12" s="6">
-        <v>33228253</v>
+        <v>33929934</v>
       </c>
       <c r="AK12" t="s">
-        <v>245</v>
+        <v>85</v>
       </c>
       <c r="AL12" t="s">
         <v>62</v>
@@ -3443,96 +3440,99 @@
         <v>64</v>
       </c>
       <c r="AO12" t="s">
-        <v>257</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3">
-        <v>44461</v>
+        <v>44427</v>
       </c>
       <c r="C13" s="3">
         <v>44635</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
         <v>67</v>
       </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" t="s">
-        <v>43</v>
-      </c>
       <c r="I13" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J13" t="s">
         <v>43</v>
       </c>
       <c r="K13" t="s">
-        <v>259</v>
+        <v>335</v>
       </c>
       <c r="L13" t="s">
-        <v>260</v>
+        <v>336</v>
       </c>
       <c r="M13" t="s">
-        <v>261</v>
+        <v>337</v>
       </c>
       <c r="N13">
         <v>2021</v>
       </c>
       <c r="O13" t="s">
-        <v>171</v>
+        <v>71</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
       </c>
       <c r="Q13" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="R13" t="s">
-        <v>262</v>
+        <v>89</v>
       </c>
       <c r="S13" t="s">
-        <v>138</v>
+        <v>247</v>
       </c>
       <c r="U13" t="s">
-        <v>263</v>
+        <v>338</v>
       </c>
       <c r="V13" t="s">
-        <v>264</v>
+        <v>339</v>
+      </c>
+      <c r="W13">
+        <v>12</v>
       </c>
       <c r="X13" t="s">
-        <v>265</v>
+        <v>340</v>
       </c>
       <c r="Y13" t="s">
-        <v>266</v>
+        <v>341</v>
       </c>
       <c r="Z13" t="s">
-        <v>125</v>
+        <v>342</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>343</v>
       </c>
       <c r="AB13" t="s">
-        <v>267</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>268</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>269</v>
+        <v>344</v>
       </c>
       <c r="AI13" t="s">
-        <v>220</v>
+        <v>345</v>
       </c>
       <c r="AJ13" s="6">
-        <v>34294425</v>
+        <v>33993265</v>
       </c>
       <c r="AK13" t="s">
-        <v>221</v>
+        <v>346</v>
       </c>
       <c r="AL13" t="s">
         <v>62</v>
@@ -3544,12 +3544,12 @@
         <v>64</v>
       </c>
       <c r="AO13" t="s">
-        <v>270</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3">
         <v>44427</v>
@@ -3573,64 +3573,76 @@
         <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J14" t="s">
         <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="L14" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="M14" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="N14">
         <v>2021</v>
       </c>
       <c r="O14" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="P14" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="Q14" t="s">
-        <v>154</v>
+        <v>285</v>
       </c>
       <c r="R14" t="s">
-        <v>121</v>
+        <v>286</v>
       </c>
       <c r="S14" t="s">
-        <v>74</v>
-      </c>
-      <c r="T14" t="s">
-        <v>276</v>
+        <v>132</v>
+      </c>
+      <c r="U14" t="s">
+        <v>287</v>
+      </c>
+      <c r="V14" t="s">
+        <v>288</v>
+      </c>
+      <c r="W14">
+        <v>21</v>
       </c>
       <c r="X14" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="Y14" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="Z14" t="s">
         <v>125</v>
       </c>
       <c r="AB14" t="s">
-        <v>279</v>
+        <v>291</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>292</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>293</v>
       </c>
       <c r="AI14" t="s">
-        <v>164</v>
+        <v>294</v>
       </c>
       <c r="AJ14" s="6">
-        <v>33471114</v>
+        <v>34010526</v>
       </c>
       <c r="AK14" t="s">
-        <v>165</v>
+        <v>295</v>
       </c>
       <c r="AL14" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="AM14" t="s">
         <v>63</v>
@@ -3639,12 +3651,12 @@
         <v>64</v>
       </c>
       <c r="AO14" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="B15" s="3">
         <v>44427</v>
@@ -3668,76 +3680,76 @@
         <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
         <v>43</v>
       </c>
       <c r="K15" t="s">
-        <v>282</v>
+        <v>348</v>
       </c>
       <c r="L15" t="s">
-        <v>283</v>
+        <v>349</v>
       </c>
       <c r="M15" t="s">
-        <v>284</v>
+        <v>350</v>
       </c>
       <c r="N15">
         <v>2021</v>
       </c>
       <c r="O15" t="s">
-        <v>153</v>
+        <v>47</v>
       </c>
       <c r="P15" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="Q15" t="s">
-        <v>285</v>
+        <v>351</v>
       </c>
       <c r="R15" t="s">
-        <v>286</v>
+        <v>352</v>
       </c>
       <c r="S15" t="s">
-        <v>132</v>
+        <v>223</v>
       </c>
       <c r="U15" t="s">
-        <v>287</v>
+        <v>353</v>
       </c>
       <c r="V15" t="s">
-        <v>288</v>
+        <v>354</v>
       </c>
       <c r="W15">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="X15" t="s">
-        <v>289</v>
+        <v>355</v>
       </c>
       <c r="Y15" t="s">
-        <v>290</v>
+        <v>356</v>
       </c>
       <c r="Z15" t="s">
         <v>125</v>
       </c>
       <c r="AB15" t="s">
-        <v>291</v>
+        <v>357</v>
       </c>
       <c r="AC15" t="s">
-        <v>292</v>
+        <v>358</v>
       </c>
       <c r="AD15" t="s">
-        <v>293</v>
+        <v>359</v>
       </c>
       <c r="AI15" t="s">
-        <v>294</v>
+        <v>360</v>
       </c>
       <c r="AJ15" s="6">
-        <v>34010526</v>
+        <v>34047758</v>
       </c>
       <c r="AK15" t="s">
-        <v>295</v>
+        <v>361</v>
       </c>
       <c r="AL15" t="s">
-        <v>98</v>
+        <v>202</v>
       </c>
       <c r="AM15" t="s">
         <v>63</v>
@@ -3746,12 +3758,12 @@
         <v>64</v>
       </c>
       <c r="AO15" t="s">
-        <v>296</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="B16" s="3">
         <v>44427</v>
@@ -3775,76 +3787,76 @@
         <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
         <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>297</v>
+        <v>168</v>
       </c>
       <c r="L16" t="s">
-        <v>298</v>
+        <v>169</v>
       </c>
       <c r="M16" t="s">
-        <v>299</v>
+        <v>170</v>
       </c>
       <c r="N16">
         <v>2021</v>
       </c>
       <c r="O16" t="s">
-        <v>300</v>
+        <v>171</v>
+      </c>
+      <c r="P16" t="s">
+        <v>132</v>
       </c>
       <c r="Q16" t="s">
-        <v>90</v>
+        <v>172</v>
       </c>
       <c r="R16" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="S16" t="s">
-        <v>132</v>
-      </c>
-      <c r="U16" t="s">
-        <v>301</v>
-      </c>
-      <c r="V16" t="s">
-        <v>302</v>
+        <v>173</v>
+      </c>
+      <c r="T16" t="s">
+        <v>174</v>
       </c>
       <c r="W16">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="X16" t="s">
-        <v>303</v>
+        <v>175</v>
       </c>
       <c r="Y16" t="s">
-        <v>304</v>
+        <v>176</v>
       </c>
       <c r="Z16" t="s">
-        <v>305</v>
+        <v>177</v>
       </c>
       <c r="AA16" t="s">
-        <v>306</v>
+        <v>178</v>
       </c>
       <c r="AB16" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="AC16" t="s">
-        <v>308</v>
+        <v>180</v>
       </c>
       <c r="AD16" t="s">
-        <v>309</v>
+        <v>181</v>
       </c>
       <c r="AI16" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="AJ16" s="6">
-        <v>33764497</v>
+        <v>34081608</v>
       </c>
       <c r="AK16" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="AL16" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="AM16" t="s">
         <v>63</v>
@@ -3853,7 +3865,7 @@
         <v>64</v>
       </c>
       <c r="AO16" t="s">
-        <v>310</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -3861,16 +3873,16 @@
         <v>41</v>
       </c>
       <c r="B17" s="3">
-        <v>44461</v>
+        <v>44427</v>
       </c>
       <c r="C17" s="3">
         <v>44635</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>43</v>
@@ -3879,70 +3891,79 @@
         <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="I17" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J17" t="s">
         <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="L17" t="s">
-        <v>312</v>
+        <v>100</v>
       </c>
       <c r="M17" t="s">
-        <v>313</v>
+        <v>101</v>
       </c>
       <c r="N17">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="O17" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+      <c r="P17" t="s">
+        <v>102</v>
       </c>
       <c r="Q17" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="R17" t="s">
-        <v>314</v>
+        <v>104</v>
       </c>
       <c r="S17" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="U17" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="V17" t="s">
-        <v>258</v>
+        <v>106</v>
+      </c>
+      <c r="W17">
+        <v>8</v>
       </c>
       <c r="X17" t="s">
-        <v>315</v>
+        <v>107</v>
       </c>
       <c r="Y17" t="s">
-        <v>316</v>
+        <v>108</v>
       </c>
       <c r="Z17" t="s">
-        <v>317</v>
+        <v>109</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>110</v>
       </c>
       <c r="AB17" t="s">
-        <v>318</v>
+        <v>111</v>
       </c>
       <c r="AC17" t="s">
-        <v>319</v>
+        <v>112</v>
       </c>
       <c r="AD17" t="s">
-        <v>320</v>
+        <v>113</v>
       </c>
       <c r="AI17" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="AJ17" s="6">
-        <v>34449885</v>
+        <v>34092431</v>
       </c>
       <c r="AK17" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="AL17" t="s">
         <v>62</v>
@@ -3954,12 +3975,12 @@
         <v>64</v>
       </c>
       <c r="AO17" t="s">
-        <v>321</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="B18" s="3">
         <v>44427</v>
@@ -3980,76 +4001,73 @@
         <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J18" t="s">
         <v>43</v>
       </c>
       <c r="K18" t="s">
-        <v>322</v>
+        <v>117</v>
       </c>
       <c r="L18" t="s">
-        <v>323</v>
+        <v>118</v>
       </c>
       <c r="M18" t="s">
-        <v>324</v>
+        <v>119</v>
       </c>
       <c r="N18">
         <v>2021</v>
       </c>
       <c r="O18" t="s">
-        <v>188</v>
+        <v>47</v>
+      </c>
+      <c r="P18" t="s">
+        <v>74</v>
       </c>
       <c r="Q18" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="R18" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="S18" t="s">
-        <v>246</v>
-      </c>
-      <c r="U18" t="s">
-        <v>325</v>
-      </c>
-      <c r="V18" t="s">
-        <v>326</v>
+        <v>50</v>
+      </c>
+      <c r="T18" t="s">
+        <v>122</v>
       </c>
       <c r="W18">
         <v>4</v>
       </c>
       <c r="X18" t="s">
-        <v>327</v>
+        <v>123</v>
       </c>
       <c r="Y18" t="s">
-        <v>328</v>
+        <v>124</v>
       </c>
       <c r="Z18" t="s">
-        <v>329</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>330</v>
+        <v>125</v>
       </c>
       <c r="AB18" t="s">
-        <v>331</v>
+        <v>126</v>
       </c>
       <c r="AC18" t="s">
-        <v>332</v>
+        <v>127</v>
       </c>
       <c r="AD18" t="s">
-        <v>333</v>
+        <v>128</v>
       </c>
       <c r="AI18" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="AJ18" s="6">
-        <v>34375655</v>
+        <v>34143195</v>
       </c>
       <c r="AK18" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="AL18" t="s">
         <v>62</v>
@@ -4061,27 +4079,27 @@
         <v>64</v>
       </c>
       <c r="AO18" t="s">
-        <v>334</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="B19" s="3">
-        <v>44427</v>
+        <v>44461</v>
       </c>
       <c r="C19" s="3">
         <v>44635</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
         <v>43</v>
@@ -4090,73 +4108,73 @@
         <v>67</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J19" t="s">
         <v>43</v>
       </c>
       <c r="K19" t="s">
-        <v>335</v>
+        <v>185</v>
       </c>
       <c r="L19" t="s">
-        <v>336</v>
+        <v>186</v>
       </c>
       <c r="M19" t="s">
-        <v>337</v>
+        <v>187</v>
       </c>
       <c r="N19">
         <v>2021</v>
       </c>
       <c r="O19" t="s">
-        <v>71</v>
-      </c>
-      <c r="P19" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="Q19" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="R19" t="s">
-        <v>89</v>
+        <v>190</v>
       </c>
       <c r="S19" t="s">
-        <v>247</v>
+        <v>132</v>
       </c>
       <c r="U19" t="s">
-        <v>338</v>
+        <v>191</v>
       </c>
       <c r="V19" t="s">
-        <v>339</v>
-      </c>
-      <c r="W19">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="X19" t="s">
-        <v>340</v>
+        <v>193</v>
       </c>
       <c r="Y19" t="s">
-        <v>341</v>
+        <v>194</v>
       </c>
       <c r="Z19" t="s">
-        <v>342</v>
+        <v>195</v>
       </c>
       <c r="AA19" t="s">
-        <v>343</v>
+        <v>196</v>
       </c>
       <c r="AB19" t="s">
-        <v>344</v>
+        <v>197</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>199</v>
       </c>
       <c r="AI19" t="s">
-        <v>345</v>
+        <v>200</v>
       </c>
       <c r="AJ19" s="6">
-        <v>33993265</v>
+        <v>34159841</v>
       </c>
       <c r="AK19" t="s">
-        <v>346</v>
+        <v>201</v>
       </c>
       <c r="AL19" t="s">
-        <v>62</v>
+        <v>202</v>
       </c>
       <c r="AM19" t="s">
         <v>63</v>
@@ -4165,15 +4183,15 @@
         <v>64</v>
       </c>
       <c r="AO19" t="s">
-        <v>347</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B20" s="3">
-        <v>44427</v>
+        <v>44449</v>
       </c>
       <c r="C20" s="3">
         <v>44635</v>
@@ -4200,70 +4218,70 @@
         <v>43</v>
       </c>
       <c r="K20" t="s">
-        <v>348</v>
+        <v>150</v>
       </c>
       <c r="L20" t="s">
-        <v>349</v>
+        <v>151</v>
       </c>
       <c r="M20" t="s">
-        <v>350</v>
+        <v>152</v>
       </c>
       <c r="N20">
         <v>2021</v>
       </c>
       <c r="O20" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="P20" t="s">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="Q20" t="s">
-        <v>351</v>
+        <v>154</v>
       </c>
       <c r="R20" t="s">
-        <v>352</v>
+        <v>121</v>
       </c>
       <c r="S20" t="s">
-        <v>223</v>
-      </c>
-      <c r="U20" t="s">
-        <v>353</v>
-      </c>
-      <c r="V20" t="s">
-        <v>354</v>
+        <v>155</v>
+      </c>
+      <c r="T20" t="s">
+        <v>156</v>
       </c>
       <c r="W20">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="X20" t="s">
-        <v>355</v>
+        <v>157</v>
       </c>
       <c r="Y20" t="s">
-        <v>356</v>
+        <v>158</v>
       </c>
       <c r="Z20" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="AB20" t="s">
-        <v>357</v>
+        <v>160</v>
       </c>
       <c r="AC20" t="s">
-        <v>358</v>
+        <v>161</v>
       </c>
       <c r="AD20" t="s">
-        <v>359</v>
+        <v>162</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>163</v>
       </c>
       <c r="AI20" t="s">
-        <v>360</v>
+        <v>164</v>
       </c>
       <c r="AJ20" s="6">
-        <v>34047758</v>
+        <v>34264327</v>
       </c>
       <c r="AK20" t="s">
-        <v>361</v>
+        <v>165</v>
       </c>
       <c r="AL20" t="s">
-        <v>202</v>
+        <v>62</v>
       </c>
       <c r="AM20" t="s">
         <v>63</v>
@@ -4272,27 +4290,27 @@
         <v>64</v>
       </c>
       <c r="AO20" t="s">
-        <v>362</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>132</v>
       </c>
       <c r="B21" s="3">
-        <v>44427</v>
+        <v>44461</v>
       </c>
       <c r="C21" s="3">
         <v>44635</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
         <v>43</v>
@@ -4307,70 +4325,73 @@
         <v>43</v>
       </c>
       <c r="K21" t="s">
-        <v>363</v>
+        <v>408</v>
       </c>
       <c r="L21" t="s">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="M21" t="s">
-        <v>365</v>
+        <v>410</v>
       </c>
       <c r="N21">
         <v>2021</v>
       </c>
       <c r="O21" t="s">
-        <v>300</v>
+        <v>171</v>
       </c>
       <c r="P21" t="s">
-        <v>204</v>
+        <v>271</v>
       </c>
       <c r="Q21" t="s">
-        <v>366</v>
+        <v>103</v>
       </c>
       <c r="R21" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="S21" t="s">
-        <v>132</v>
+        <v>411</v>
       </c>
       <c r="U21" t="s">
-        <v>367</v>
+        <v>412</v>
       </c>
       <c r="V21" t="s">
-        <v>368</v>
+        <v>413</v>
       </c>
       <c r="W21">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>369</v>
+        <v>414</v>
       </c>
       <c r="Y21" t="s">
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="Z21" t="s">
-        <v>371</v>
+        <v>416</v>
       </c>
       <c r="AA21" t="s">
-        <v>372</v>
+        <v>417</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>418</v>
       </c>
       <c r="AC21" t="s">
-        <v>373</v>
+        <v>419</v>
       </c>
       <c r="AD21" t="s">
-        <v>374</v>
+        <v>420</v>
       </c>
       <c r="AE21" t="s">
-        <v>375</v>
+        <v>421</v>
       </c>
       <c r="AI21" t="s">
-        <v>376</v>
+        <v>114</v>
       </c>
       <c r="AJ21" s="6">
-        <v>33870242</v>
+        <v>34274126</v>
       </c>
       <c r="AK21" t="s">
-        <v>377</v>
+        <v>103</v>
       </c>
       <c r="AL21" t="s">
         <v>62</v>
@@ -4382,27 +4403,27 @@
         <v>64</v>
       </c>
       <c r="AO21" t="s">
-        <v>378</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B22" s="3">
-        <v>44427</v>
+        <v>44461</v>
       </c>
       <c r="C22" s="3">
         <v>44635</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
         <v>43</v>
@@ -4417,70 +4438,61 @@
         <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>379</v>
+        <v>259</v>
       </c>
       <c r="L22" t="s">
-        <v>380</v>
+        <v>260</v>
       </c>
       <c r="M22" t="s">
-        <v>381</v>
+        <v>261</v>
       </c>
       <c r="N22">
         <v>2021</v>
       </c>
       <c r="O22" t="s">
-        <v>188</v>
-      </c>
-      <c r="P22" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
       <c r="Q22" t="s">
-        <v>382</v>
+        <v>208</v>
       </c>
       <c r="R22" t="s">
-        <v>97</v>
+        <v>262</v>
       </c>
       <c r="S22" t="s">
-        <v>74</v>
-      </c>
-      <c r="T22" t="s">
-        <v>96</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
+        <v>138</v>
+      </c>
+      <c r="U22" t="s">
+        <v>263</v>
+      </c>
+      <c r="V22" t="s">
+        <v>264</v>
       </c>
       <c r="X22" t="s">
-        <v>383</v>
+        <v>265</v>
       </c>
       <c r="Y22" t="s">
-        <v>384</v>
+        <v>266</v>
       </c>
       <c r="Z22" t="s">
-        <v>385</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>386</v>
+        <v>125</v>
       </c>
       <c r="AB22" t="s">
-        <v>387</v>
+        <v>267</v>
       </c>
       <c r="AC22" t="s">
-        <v>388</v>
+        <v>268</v>
       </c>
       <c r="AD22" t="s">
-        <v>389</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>390</v>
+        <v>269</v>
       </c>
       <c r="AI22" t="s">
-        <v>391</v>
+        <v>220</v>
       </c>
       <c r="AJ22" s="6">
-        <v>34465306</v>
+        <v>34294425</v>
       </c>
       <c r="AK22" t="s">
-        <v>392</v>
+        <v>221</v>
       </c>
       <c r="AL22" t="s">
         <v>62</v>
@@ -4492,7 +4504,7 @@
         <v>64</v>
       </c>
       <c r="AO22" t="s">
-        <v>393</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -4521,76 +4533,73 @@
         <v>67</v>
       </c>
       <c r="I23" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J23" t="s">
         <v>43</v>
       </c>
       <c r="K23" t="s">
-        <v>394</v>
+        <v>322</v>
       </c>
       <c r="L23" t="s">
-        <v>395</v>
+        <v>323</v>
       </c>
       <c r="M23" t="s">
-        <v>396</v>
+        <v>324</v>
       </c>
       <c r="N23">
         <v>2021</v>
       </c>
       <c r="O23" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="Q23" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="R23" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="S23" t="s">
-        <v>173</v>
+        <v>246</v>
       </c>
       <c r="U23" t="s">
-        <v>397</v>
+        <v>325</v>
       </c>
       <c r="V23" t="s">
-        <v>398</v>
+        <v>326</v>
       </c>
       <c r="W23">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="X23" t="s">
-        <v>399</v>
+        <v>327</v>
       </c>
       <c r="Y23" t="s">
-        <v>400</v>
+        <v>328</v>
       </c>
       <c r="Z23" t="s">
-        <v>401</v>
+        <v>329</v>
       </c>
       <c r="AA23" t="s">
-        <v>402</v>
+        <v>330</v>
       </c>
       <c r="AB23" t="s">
-        <v>403</v>
+        <v>331</v>
       </c>
       <c r="AC23" t="s">
-        <v>404</v>
+        <v>332</v>
       </c>
       <c r="AD23" t="s">
-        <v>405</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>406</v>
+        <v>333</v>
       </c>
       <c r="AI23" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="AJ23" s="6">
-        <v>33861873</v>
+        <v>34375655</v>
       </c>
       <c r="AK23" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AL23" t="s">
         <v>62</v>
@@ -4602,12 +4611,12 @@
         <v>64</v>
       </c>
       <c r="AO23" t="s">
-        <v>407</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="B24" s="3">
         <v>44461</v>
@@ -4622,7 +4631,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
         <v>43</v>
@@ -4637,73 +4646,61 @@
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>408</v>
+        <v>311</v>
       </c>
       <c r="L24" t="s">
-        <v>409</v>
+        <v>312</v>
       </c>
       <c r="M24" t="s">
-        <v>410</v>
+        <v>313</v>
       </c>
       <c r="N24">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="O24" t="s">
-        <v>171</v>
-      </c>
-      <c r="P24" t="s">
-        <v>271</v>
+        <v>95</v>
       </c>
       <c r="Q24" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="R24" t="s">
-        <v>104</v>
+        <v>314</v>
       </c>
       <c r="S24" t="s">
-        <v>411</v>
+        <v>74</v>
       </c>
       <c r="U24" t="s">
-        <v>412</v>
+        <v>173</v>
       </c>
       <c r="V24" t="s">
-        <v>413</v>
-      </c>
-      <c r="W24">
-        <v>1</v>
+        <v>258</v>
       </c>
       <c r="X24" t="s">
-        <v>414</v>
+        <v>315</v>
       </c>
       <c r="Y24" t="s">
-        <v>415</v>
+        <v>316</v>
       </c>
       <c r="Z24" t="s">
-        <v>416</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>417</v>
+        <v>317</v>
       </c>
       <c r="AB24" t="s">
-        <v>418</v>
+        <v>318</v>
       </c>
       <c r="AC24" t="s">
-        <v>419</v>
+        <v>319</v>
       </c>
       <c r="AD24" t="s">
-        <v>420</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>421</v>
+        <v>320</v>
       </c>
       <c r="AI24" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="AJ24" s="6">
-        <v>34274126</v>
+        <v>34449885</v>
       </c>
       <c r="AK24" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="AL24" t="s">
         <v>62</v>
@@ -4715,12 +4712,12 @@
         <v>64</v>
       </c>
       <c r="AO24" t="s">
-        <v>422</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="B25" s="3">
         <v>44427</v>
@@ -4738,79 +4735,76 @@
         <v>43</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H25" t="s">
         <v>67</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="J25" t="s">
         <v>43</v>
       </c>
       <c r="K25" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="L25" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="M25" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="N25">
         <v>2021</v>
       </c>
       <c r="O25" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="Q25" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="R25" t="s">
-        <v>258</v>
+        <v>441</v>
       </c>
       <c r="S25" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="U25" t="s">
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="V25" t="s">
-        <v>428</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
+        <v>443</v>
       </c>
       <c r="X25" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="Y25" t="s">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="Z25" t="s">
         <v>125</v>
       </c>
       <c r="AB25" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="AC25" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="AD25" t="s">
-        <v>433</v>
+        <v>448</v>
       </c>
       <c r="AI25" t="s">
-        <v>434</v>
+        <v>449</v>
       </c>
       <c r="AJ25" s="6">
-        <v>33577743</v>
+        <v>34464194</v>
       </c>
       <c r="AK25" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="AL25" t="s">
-        <v>94</v>
+        <v>451</v>
       </c>
       <c r="AM25" t="s">
         <v>63</v>
@@ -4819,12 +4813,12 @@
         <v>64</v>
       </c>
       <c r="AO25" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>244</v>
+        <v>73</v>
       </c>
       <c r="B26" s="3">
         <v>44427</v>
@@ -4842,76 +4836,85 @@
         <v>43</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="I26" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J26" t="s">
         <v>43</v>
       </c>
       <c r="K26" t="s">
-        <v>437</v>
+        <v>379</v>
       </c>
       <c r="L26" t="s">
-        <v>438</v>
+        <v>380</v>
       </c>
       <c r="M26" t="s">
-        <v>439</v>
+        <v>381</v>
       </c>
       <c r="N26">
         <v>2021</v>
       </c>
       <c r="O26" t="s">
-        <v>171</v>
+        <v>188</v>
+      </c>
+      <c r="P26" t="s">
+        <v>74</v>
       </c>
       <c r="Q26" t="s">
-        <v>440</v>
+        <v>382</v>
       </c>
       <c r="R26" t="s">
-        <v>441</v>
+        <v>97</v>
       </c>
       <c r="S26" t="s">
-        <v>173</v>
-      </c>
-      <c r="U26" t="s">
-        <v>442</v>
-      </c>
-      <c r="V26" t="s">
-        <v>443</v>
+        <v>74</v>
+      </c>
+      <c r="T26" t="s">
+        <v>96</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
       </c>
       <c r="X26" t="s">
-        <v>444</v>
+        <v>383</v>
       </c>
       <c r="Y26" t="s">
-        <v>445</v>
+        <v>384</v>
       </c>
       <c r="Z26" t="s">
-        <v>125</v>
+        <v>385</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>386</v>
       </c>
       <c r="AB26" t="s">
-        <v>446</v>
+        <v>387</v>
       </c>
       <c r="AC26" t="s">
-        <v>447</v>
+        <v>388</v>
       </c>
       <c r="AD26" t="s">
-        <v>448</v>
+        <v>389</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>390</v>
       </c>
       <c r="AI26" t="s">
-        <v>449</v>
+        <v>391</v>
       </c>
       <c r="AJ26" s="6">
-        <v>34464194</v>
+        <v>34465306</v>
       </c>
       <c r="AK26" t="s">
-        <v>450</v>
+        <v>392</v>
       </c>
       <c r="AL26" t="s">
-        <v>451</v>
+        <v>62</v>
       </c>
       <c r="AM26" t="s">
         <v>63</v>
@@ -4920,7 +4923,7 @@
         <v>64</v>
       </c>
       <c r="AO26" t="s">
-        <v>452</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5850,15 +5853,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF80A72F950AB44BBD3F7B6758C7B51D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b571fce440275f0622ff001093cb92ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111" xmlns:ns3="e5c03532-ca69-4eca-baa0-f6c5bcd6c094" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f94315dc4d15cb105dea15baff015bd0" ns2:_="" ns3:_="">
     <xsd:import namespace="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111"/>
@@ -6077,6 +6071,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6089,14 +6092,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E8C1E19-A830-4B1D-A214-DB562C43BEFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C88EE5-86E9-41E8-B78D-87883268C3C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6115,6 +6110,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E8C1E19-A830-4B1D-A214-DB562C43BEFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CA334D6-291A-41FC-A9C5-B3FB328B715B}">
   <ds:schemaRefs>

</xml_diff>